<commit_message>
modified:   main.ipynb 	modified:   predictBySARIMA.xlsx 	modified:   pythonCode/SARIMAprocesser.py 	modified:   pythonCode/__pycache__/SARIMAprocesser.cpython-39.pyc 	new file:   test/ForestcastUnivariate.ipynb
</commit_message>
<xml_diff>
--- a/predictBySARIMA.xlsx
+++ b/predictBySARIMA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>NO</t>
   </si>
@@ -41,6 +41,42 @@
   </si>
   <si>
     <t>Temp</t>
+  </si>
+  <si>
+    <t>Barometer</t>
+  </si>
+  <si>
+    <t>Radiation</t>
+  </si>
+  <si>
+    <t>WindDir</t>
+  </si>
+  <si>
+    <t>SO2</t>
+  </si>
+  <si>
+    <t>Compass</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>Wind Spd</t>
+  </si>
+  <si>
+    <t>Hướng gió</t>
+  </si>
+  <si>
+    <t>Nhiệt độ</t>
+  </si>
+  <si>
+    <t>Áp suất khí quyển</t>
+  </si>
+  <si>
+    <t>Wind Spd (sai)</t>
   </si>
   <si>
     <t>time</t>
@@ -407,15 +443,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:V49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -444,8 +480,44 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" s="2">
         <v>43713.29166666666</v>
       </c>
@@ -476,8 +548,44 @@
       <c r="J2">
         <v>27.68966433459666</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <v>1008.308089706799</v>
+      </c>
+      <c r="L2">
+        <v>3.090161378250816</v>
+      </c>
+      <c r="M2">
+        <v>161.5009957280141</v>
+      </c>
+      <c r="N2">
+        <v>78.10731194144161</v>
+      </c>
+      <c r="O2">
+        <v>323.1092944001313</v>
+      </c>
+      <c r="P2">
+        <v>274.2591695244</v>
+      </c>
+      <c r="Q2">
+        <v>65.07842994580639</v>
+      </c>
+      <c r="R2">
+        <v>0.8250339349143578</v>
+      </c>
+      <c r="S2">
+        <v>248.961452954344</v>
+      </c>
+      <c r="T2">
+        <v>27.76460958939195</v>
+      </c>
+      <c r="U2">
+        <v>1002.085139192587</v>
+      </c>
+      <c r="V2">
+        <v>1.432750677088185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" s="2">
         <v>43713.33333333334</v>
       </c>
@@ -508,8 +616,44 @@
       <c r="J3">
         <v>24.92763202924905</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3">
+        <v>1007.12732780073</v>
+      </c>
+      <c r="L3">
+        <v>36.7531698152215</v>
+      </c>
+      <c r="M3">
+        <v>161.280747219477</v>
+      </c>
+      <c r="N3">
+        <v>73.52409811207978</v>
+      </c>
+      <c r="O3">
+        <v>323.0807015064688</v>
+      </c>
+      <c r="P3">
+        <v>316.1224758706166</v>
+      </c>
+      <c r="Q3">
+        <v>62.31421358907601</v>
+      </c>
+      <c r="R3">
+        <v>1.450358416169506</v>
+      </c>
+      <c r="S3">
+        <v>204.3018921809876</v>
+      </c>
+      <c r="T3">
+        <v>27.03721897015934</v>
+      </c>
+      <c r="U3">
+        <v>1001.978518165466</v>
+      </c>
+      <c r="V3">
+        <v>1.069333962011558</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" s="2">
         <v>43713.375</v>
       </c>
@@ -540,8 +684,44 @@
       <c r="J4">
         <v>27.16989080740736</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <v>1006.37354239926</v>
+      </c>
+      <c r="L4">
+        <v>119.7723303809588</v>
+      </c>
+      <c r="M4">
+        <v>172.9350846706085</v>
+      </c>
+      <c r="N4">
+        <v>73.57879065176336</v>
+      </c>
+      <c r="O4">
+        <v>322.9570584031585</v>
+      </c>
+      <c r="P4">
+        <v>369.7958631781835</v>
+      </c>
+      <c r="Q4">
+        <v>62.13803835927827</v>
+      </c>
+      <c r="R4">
+        <v>1.146651811016817</v>
+      </c>
+      <c r="S4">
+        <v>159.1714327200366</v>
+      </c>
+      <c r="T4">
+        <v>26.38588615079973</v>
+      </c>
+      <c r="U4">
+        <v>1003.472336172717</v>
+      </c>
+      <c r="V4">
+        <v>1.555768617849526</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="2">
         <v>43713.41666666666</v>
       </c>
@@ -572,8 +752,44 @@
       <c r="J5">
         <v>26.06926491443312</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5">
+        <v>1005.830706978364</v>
+      </c>
+      <c r="L5">
+        <v>206.8402024788217</v>
+      </c>
+      <c r="M5">
+        <v>147.275991642498</v>
+      </c>
+      <c r="N5">
+        <v>71.54273763234569</v>
+      </c>
+      <c r="O5">
+        <v>323.1513547083603</v>
+      </c>
+      <c r="P5">
+        <v>325.6929192077124</v>
+      </c>
+      <c r="Q5">
+        <v>64.29061337078025</v>
+      </c>
+      <c r="R5">
+        <v>1.969633920420697</v>
+      </c>
+      <c r="S5">
+        <v>129.309632304436</v>
+      </c>
+      <c r="T5">
+        <v>26.11480460638244</v>
+      </c>
+      <c r="U5">
+        <v>1003.717268357919</v>
+      </c>
+      <c r="V5">
+        <v>1.556596426879973</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="2">
         <v>43713.45833333334</v>
       </c>
@@ -604,8 +820,44 @@
       <c r="J6">
         <v>25.0738232420867</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6">
+        <v>1008.423180765203</v>
+      </c>
+      <c r="L6">
+        <v>300.4404948644899</v>
+      </c>
+      <c r="M6">
+        <v>138.3715165707952</v>
+      </c>
+      <c r="N6">
+        <v>70.72381234831963</v>
+      </c>
+      <c r="O6">
+        <v>323.1219158742389</v>
+      </c>
+      <c r="P6">
+        <v>300.6141682576495</v>
+      </c>
+      <c r="Q6">
+        <v>68.74140763733354</v>
+      </c>
+      <c r="R6">
+        <v>1.512425542464811</v>
+      </c>
+      <c r="S6">
+        <v>148.7736371642254</v>
+      </c>
+      <c r="T6">
+        <v>26.18319233014082</v>
+      </c>
+      <c r="U6">
+        <v>1003.75108476871</v>
+      </c>
+      <c r="V6">
+        <v>1.184927249994621</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="2">
         <v>43713.5</v>
       </c>
@@ -636,8 +888,44 @@
       <c r="J7">
         <v>29.83208755179922</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7">
+        <v>1007.145397281524</v>
+      </c>
+      <c r="L7">
+        <v>397.2500420615611</v>
+      </c>
+      <c r="M7">
+        <v>157.4313942286694</v>
+      </c>
+      <c r="N7">
+        <v>69.97428810912949</v>
+      </c>
+      <c r="O7">
+        <v>322.9745286818052</v>
+      </c>
+      <c r="P7">
+        <v>306.1263039817781</v>
+      </c>
+      <c r="Q7">
+        <v>71.9731247225874</v>
+      </c>
+      <c r="R7">
+        <v>1.48226509476524</v>
+      </c>
+      <c r="S7">
+        <v>145.8430119705236</v>
+      </c>
+      <c r="T7">
+        <v>26.03875714400815</v>
+      </c>
+      <c r="U7">
+        <v>1002.974604324435</v>
+      </c>
+      <c r="V7">
+        <v>1.1073428960882</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="2">
         <v>43713.54166666666</v>
       </c>
@@ -668,8 +956,44 @@
       <c r="J8">
         <v>27.86809083736143</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8">
+        <v>1007.494229565005</v>
+      </c>
+      <c r="L8">
+        <v>536.5299560264493</v>
+      </c>
+      <c r="M8">
+        <v>151.163056064791</v>
+      </c>
+      <c r="N8">
+        <v>70.040419296244</v>
+      </c>
+      <c r="O8">
+        <v>322.79770265525</v>
+      </c>
+      <c r="P8">
+        <v>290.6738033484028</v>
+      </c>
+      <c r="Q8">
+        <v>72.97857422861009</v>
+      </c>
+      <c r="R8">
+        <v>1.50557075095209</v>
+      </c>
+      <c r="S8">
+        <v>132.251401880447</v>
+      </c>
+      <c r="T8">
+        <v>25.70167393121404</v>
+      </c>
+      <c r="U8">
+        <v>1001.442771023199</v>
+      </c>
+      <c r="V8">
+        <v>1.406265602192108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="2">
         <v>43713.58333333334</v>
       </c>
@@ -700,8 +1024,44 @@
       <c r="J9">
         <v>28.93158447695653</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9">
+        <v>1007.588222258847</v>
+      </c>
+      <c r="L9">
+        <v>476.9610495767927</v>
+      </c>
+      <c r="M9">
+        <v>126.1417158402301</v>
+      </c>
+      <c r="N9">
+        <v>70.27426639578374</v>
+      </c>
+      <c r="O9">
+        <v>322.9745286818052</v>
+      </c>
+      <c r="P9">
+        <v>278.980416040836</v>
+      </c>
+      <c r="Q9">
+        <v>72.41426719216118</v>
+      </c>
+      <c r="R9">
+        <v>1.726492561722923</v>
+      </c>
+      <c r="S9">
+        <v>162.9685407025778</v>
+      </c>
+      <c r="T9">
+        <v>25.31026366129106</v>
+      </c>
+      <c r="U9">
+        <v>1001.116599657018</v>
+      </c>
+      <c r="V9">
+        <v>1.220393645926833</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="2">
         <v>43713.625</v>
       </c>
@@ -732,8 +1092,44 @@
       <c r="J10">
         <v>27.91735405482232</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10">
+        <v>1007.136342705608</v>
+      </c>
+      <c r="L10">
+        <v>431.1540814824725</v>
+      </c>
+      <c r="M10">
+        <v>137.2802763602062</v>
+      </c>
+      <c r="N10">
+        <v>70.78639300948933</v>
+      </c>
+      <c r="O10">
+        <v>323.0512626723473</v>
+      </c>
+      <c r="P10">
+        <v>288.3683587445565</v>
+      </c>
+      <c r="Q10">
+        <v>71.20523621502531</v>
+      </c>
+      <c r="R10">
+        <v>0.8405529248008647</v>
+      </c>
+      <c r="S10">
+        <v>189.0403998390667</v>
+      </c>
+      <c r="T10">
+        <v>24.77141309244143</v>
+      </c>
+      <c r="U10">
+        <v>1001.191915628309</v>
+      </c>
+      <c r="V10">
+        <v>0.9601670545753667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="2">
         <v>43713.66666666666</v>
       </c>
@@ -764,8 +1160,44 @@
       <c r="J11">
         <v>28.27381972669247</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11">
+        <v>1007.029204791836</v>
+      </c>
+      <c r="L11">
+        <v>404.8402146781052</v>
+      </c>
+      <c r="M11">
+        <v>106.1715401058593</v>
+      </c>
+      <c r="N11">
+        <v>71.61499033780142</v>
+      </c>
+      <c r="O11">
+        <v>322.5447217036315</v>
+      </c>
+      <c r="P11">
+        <v>292.3708593779318</v>
+      </c>
+      <c r="Q11">
+        <v>72.89927975185763</v>
+      </c>
+      <c r="R11">
+        <v>1.920951154305667</v>
+      </c>
+      <c r="S11">
+        <v>198.383697352636</v>
+      </c>
+      <c r="T11">
+        <v>24.00837402805548</v>
+      </c>
+      <c r="U11">
+        <v>1000.495432973636</v>
+      </c>
+      <c r="V11">
+        <v>1.31348252808485</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="2">
         <v>43713.70833333334</v>
       </c>
@@ -796,8 +1228,44 @@
       <c r="J12">
         <v>26.19842306893561</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12">
+        <v>1004.638595448395</v>
+      </c>
+      <c r="L12">
+        <v>315.2149889295728</v>
+      </c>
+      <c r="M12">
+        <v>156.5558876697332</v>
+      </c>
+      <c r="N12">
+        <v>71.85079825533883</v>
+      </c>
+      <c r="O12">
+        <v>322.4593951026857</v>
+      </c>
+      <c r="P12">
+        <v>288.6166663575236</v>
+      </c>
+      <c r="Q12">
+        <v>75.04173350045863</v>
+      </c>
+      <c r="R12">
+        <v>1.887621792983717</v>
+      </c>
+      <c r="S12">
+        <v>196.7148833000698</v>
+      </c>
+      <c r="T12">
+        <v>23.11783459136901</v>
+      </c>
+      <c r="U12">
+        <v>1000.040548492614</v>
+      </c>
+      <c r="V12">
+        <v>1.24951141525444</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="2">
         <v>43713.75</v>
       </c>
@@ -828,8 +1296,44 @@
       <c r="J13">
         <v>25.16106531914484</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13">
+        <v>1005.552040658211</v>
+      </c>
+      <c r="L13">
+        <v>113.6564934460374</v>
+      </c>
+      <c r="M13">
+        <v>167.2623445979606</v>
+      </c>
+      <c r="N13">
+        <v>71.50928906734627</v>
+      </c>
+      <c r="O13">
+        <v>322.5147217036315</v>
+      </c>
+      <c r="P13">
+        <v>324.9071096946194</v>
+      </c>
+      <c r="Q13">
+        <v>75.3797792334281</v>
+      </c>
+      <c r="R13">
+        <v>1.549915907457272</v>
+      </c>
+      <c r="S13">
+        <v>203.6596299170916</v>
+      </c>
+      <c r="T13">
+        <v>21.93623003117754</v>
+      </c>
+      <c r="U13">
+        <v>999.9048089028987</v>
+      </c>
+      <c r="V13">
+        <v>1.465095146977746</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="2">
         <v>43713.79166666666</v>
       </c>
@@ -860,8 +1364,44 @@
       <c r="J14">
         <v>28.40384945548674</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14">
+        <v>1008.96438336188</v>
+      </c>
+      <c r="L14">
+        <v>44.83416843946436</v>
+      </c>
+      <c r="M14">
+        <v>170.5925030122315</v>
+      </c>
+      <c r="N14">
+        <v>72.46583724907946</v>
+      </c>
+      <c r="O14">
+        <v>322.9864972372801</v>
+      </c>
+      <c r="P14">
+        <v>370.0938008149017</v>
+      </c>
+      <c r="Q14">
+        <v>77.02848755133567</v>
+      </c>
+      <c r="R14">
+        <v>1.606735910868807</v>
+      </c>
+      <c r="S14">
+        <v>173.3974467884574</v>
+      </c>
+      <c r="T14">
+        <v>20.36095152411215</v>
+      </c>
+      <c r="U14">
+        <v>1000.722716790532</v>
+      </c>
+      <c r="V14">
+        <v>1.326212643347811</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="2">
         <v>43713.83333333334</v>
       </c>
@@ -892,8 +1432,44 @@
       <c r="J15">
         <v>24.94074955347645</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15">
+        <v>1010.293410631862</v>
+      </c>
+      <c r="L15">
+        <v>11.6169958909596</v>
+      </c>
+      <c r="M15">
+        <v>155.1360982679354</v>
+      </c>
+      <c r="N15">
+        <v>74.11831495799699</v>
+      </c>
+      <c r="O15">
+        <v>322.7313547083604</v>
+      </c>
+      <c r="P15">
+        <v>422.9812192201761</v>
+      </c>
+      <c r="Q15">
+        <v>78.80124769891724</v>
+      </c>
+      <c r="R15">
+        <v>1.412663170801402</v>
+      </c>
+      <c r="S15">
+        <v>182.4689712282027</v>
+      </c>
+      <c r="T15">
+        <v>18.80958857104</v>
+      </c>
+      <c r="U15">
+        <v>1000.340317229625</v>
+      </c>
+      <c r="V15">
+        <v>1.326469300037262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="2">
         <v>43713.875</v>
       </c>
@@ -924,8 +1500,44 @@
       <c r="J16">
         <v>27.95405987013652</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16">
+        <v>1007.946043212782</v>
+      </c>
+      <c r="L16">
+        <v>-0.0009215258612470336</v>
+      </c>
+      <c r="M16">
+        <v>117.5405351865127</v>
+      </c>
+      <c r="N16">
+        <v>74.47796120428532</v>
+      </c>
+      <c r="O16">
+        <v>322.7313547083604</v>
+      </c>
+      <c r="P16">
+        <v>328.4179154074607</v>
+      </c>
+      <c r="Q16">
+        <v>78.96220965928109</v>
+      </c>
+      <c r="R16">
+        <v>1.912198209926392</v>
+      </c>
+      <c r="S16">
+        <v>161.5269596144907</v>
+      </c>
+      <c r="T16">
+        <v>17.68318556138864</v>
+      </c>
+      <c r="U16">
+        <v>1000.121104605454</v>
+      </c>
+      <c r="V16">
+        <v>1.355611217327061</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" s="2">
         <v>43713.91666666666</v>
       </c>
@@ -956,8 +1568,44 @@
       <c r="J17">
         <v>29.73529005087723</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17">
+        <v>1007.91818204589</v>
+      </c>
+      <c r="L17">
+        <v>-0.0008248833807180495</v>
+      </c>
+      <c r="M17">
+        <v>133.3116800370068</v>
+      </c>
+      <c r="N17">
+        <v>75.1723942913962</v>
+      </c>
+      <c r="O17">
+        <v>322.9040685017399</v>
+      </c>
+      <c r="P17">
+        <v>275.5304970021863</v>
+      </c>
+      <c r="Q17">
+        <v>80.12765593498457</v>
+      </c>
+      <c r="R17">
+        <v>1.452868671123206</v>
+      </c>
+      <c r="S17">
+        <v>153.4042746658376</v>
+      </c>
+      <c r="T17">
+        <v>16.7630410844138</v>
+      </c>
+      <c r="U17">
+        <v>1000.422580780479</v>
+      </c>
+      <c r="V17">
+        <v>1.90881171298952</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" s="2">
         <v>43713.95833333334</v>
       </c>
@@ -988,8 +1636,44 @@
       <c r="J18">
         <v>27.07548299174217</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18">
+        <v>1005.684858987648</v>
+      </c>
+      <c r="L18">
+        <v>-0.0009117997294605301</v>
+      </c>
+      <c r="M18">
+        <v>128.7754486683313</v>
+      </c>
+      <c r="N18">
+        <v>76.39932709822423</v>
+      </c>
+      <c r="O18">
+        <v>322.8746296676184</v>
+      </c>
+      <c r="P18">
+        <v>271.7763039817781</v>
+      </c>
+      <c r="Q18">
+        <v>78.60721254892511</v>
+      </c>
+      <c r="R18">
+        <v>1.325821713265118</v>
+      </c>
+      <c r="S18">
+        <v>144.1640473389066</v>
+      </c>
+      <c r="T18">
+        <v>15.87619237213449</v>
+      </c>
+      <c r="U18">
+        <v>1002.064400004099</v>
+      </c>
+      <c r="V18">
+        <v>1.897903871558369</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" s="2">
         <v>43714</v>
       </c>
@@ -1020,8 +1704,44 @@
       <c r="J19">
         <v>28.51074052438492</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19">
+        <v>1008.122707930776</v>
+      </c>
+      <c r="L19">
+        <v>-0.0009042675037995025</v>
+      </c>
+      <c r="M19">
+        <v>108.1143800291865</v>
+      </c>
+      <c r="N19">
+        <v>74.95262469675409</v>
+      </c>
+      <c r="O19">
+        <v>323.1513547083604</v>
+      </c>
+      <c r="P19">
+        <v>262.079166990899</v>
+      </c>
+      <c r="Q19">
+        <v>76.48510063081459</v>
+      </c>
+      <c r="R19">
+        <v>2.015464178183486</v>
+      </c>
+      <c r="S19">
+        <v>134.7219161009102</v>
+      </c>
+      <c r="T19">
+        <v>14.89841255812641</v>
+      </c>
+      <c r="U19">
+        <v>1002.477683368232</v>
+      </c>
+      <c r="V19">
+        <v>1.536344818895624</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" s="2">
         <v>43714.04166666666</v>
       </c>
@@ -1052,8 +1772,44 @@
       <c r="J20">
         <v>29.18555195150538</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20">
+        <v>1006.502555247439</v>
+      </c>
+      <c r="L20">
+        <v>-0.000664540963877287</v>
+      </c>
+      <c r="M20">
+        <v>136.6671963921543</v>
+      </c>
+      <c r="N20">
+        <v>72.72143551841361</v>
+      </c>
+      <c r="O20">
+        <v>323.1513547083604</v>
+      </c>
+      <c r="P20">
+        <v>239.1233600113071</v>
+      </c>
+      <c r="Q20">
+        <v>73.79223624250211</v>
+      </c>
+      <c r="R20">
+        <v>1.221592268887455</v>
+      </c>
+      <c r="S20">
+        <v>166.918987086132</v>
+      </c>
+      <c r="T20">
+        <v>13.83178825383002</v>
+      </c>
+      <c r="U20">
+        <v>1001.177296483481</v>
+      </c>
+      <c r="V20">
+        <v>1.329320833096976</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" s="2">
         <v>43714.08333333334</v>
       </c>
@@ -1084,8 +1840,44 @@
       <c r="J21">
         <v>27.81354873552966</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21">
+        <v>1005.657169956086</v>
+      </c>
+      <c r="L21">
+        <v>-0.0004979102052956082</v>
+      </c>
+      <c r="M21">
+        <v>147.5761676134835</v>
+      </c>
+      <c r="N21">
+        <v>71.12826337171228</v>
+      </c>
+      <c r="O21">
+        <v>323.1513547083604</v>
+      </c>
+      <c r="P21">
+        <v>252.9954982689369</v>
+      </c>
+      <c r="Q21">
+        <v>69.47682323986068</v>
+      </c>
+      <c r="R21">
+        <v>1.165229850008925</v>
+      </c>
+      <c r="S21">
+        <v>186.239548103218</v>
+      </c>
+      <c r="T21">
+        <v>12.40464080572968</v>
+      </c>
+      <c r="U21">
+        <v>999.8012599197973</v>
+      </c>
+      <c r="V21">
+        <v>0.9927925904171534</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
       <c r="A22" s="2">
         <v>43714.125</v>
       </c>
@@ -1116,8 +1908,44 @@
       <c r="J22">
         <v>27.38964068858418</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22">
+        <v>1005.755167469662</v>
+      </c>
+      <c r="L22">
+        <v>-0.002391355429977902</v>
+      </c>
+      <c r="M22">
+        <v>142.5146897700074</v>
+      </c>
+      <c r="N22">
+        <v>72.19162904575745</v>
+      </c>
+      <c r="O22">
+        <v>323.1513547083604</v>
+      </c>
+      <c r="P22">
+        <v>241.4846115947453</v>
+      </c>
+      <c r="Q22">
+        <v>68.94795582732722</v>
+      </c>
+      <c r="R22">
+        <v>1.325942687023449</v>
+      </c>
+      <c r="S22">
+        <v>157.3777177626899</v>
+      </c>
+      <c r="T22">
+        <v>11.6715219374151</v>
+      </c>
+      <c r="U22">
+        <v>1000.542589932916</v>
+      </c>
+      <c r="V22">
+        <v>1.265757363996033</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23" s="2">
         <v>43714.16666666666</v>
       </c>
@@ -1148,8 +1976,44 @@
       <c r="J23">
         <v>26.12613698166167</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23">
+        <v>1005.747767279574</v>
+      </c>
+      <c r="L23">
+        <v>-0.0002550436601309926</v>
+      </c>
+      <c r="M23">
+        <v>137.1688824052269</v>
+      </c>
+      <c r="N23">
+        <v>73.47583495365213</v>
+      </c>
+      <c r="O23">
+        <v>323.1513547083604</v>
+      </c>
+      <c r="P23">
+        <v>226.0321109613701</v>
+      </c>
+      <c r="Q23">
+        <v>71.11927859746559</v>
+      </c>
+      <c r="R23">
+        <v>1.55956906054124</v>
+      </c>
+      <c r="S23">
+        <v>135.3547094326842</v>
+      </c>
+      <c r="T23">
+        <v>11.0277013688684</v>
+      </c>
+      <c r="U23">
+        <v>1000.683372699432</v>
+      </c>
+      <c r="V23">
+        <v>1.456882293496734</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24" s="2">
         <v>43714.20833333334</v>
       </c>
@@ -1180,8 +2044,44 @@
       <c r="J24">
         <v>28.13393956981811</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24">
+        <v>1007.078451405828</v>
+      </c>
+      <c r="L24">
+        <v>-0.0001387684332245528</v>
+      </c>
+      <c r="M24">
+        <v>172.3558866670889</v>
+      </c>
+      <c r="N24">
+        <v>72.72514612473313</v>
+      </c>
+      <c r="O24">
+        <v>323.1513547083604</v>
+      </c>
+      <c r="P24">
+        <v>237.48211096137</v>
+      </c>
+      <c r="Q24">
+        <v>70.52795170093461</v>
+      </c>
+      <c r="R24">
+        <v>1.193896885649003</v>
+      </c>
+      <c r="S24">
+        <v>126.0339129696055</v>
+      </c>
+      <c r="T24">
+        <v>10.06161921896131</v>
+      </c>
+      <c r="U24">
+        <v>1001.233472233939</v>
+      </c>
+      <c r="V24">
+        <v>1.148304964082062</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
       <c r="A25" s="2">
         <v>43714.25</v>
       </c>
@@ -1212,8 +2112,44 @@
       <c r="J25">
         <v>26.49642860914965</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25">
+        <v>1007.461590014075</v>
+      </c>
+      <c r="L25">
+        <v>-8.314618588944455E-05</v>
+      </c>
+      <c r="M25">
+        <v>134.5679036915914</v>
+      </c>
+      <c r="N25">
+        <v>75.20396788917884</v>
+      </c>
+      <c r="O25">
+        <v>323.1513547083604</v>
+      </c>
+      <c r="P25">
+        <v>286.128721120302</v>
+      </c>
+      <c r="Q25">
+        <v>65.07937307866118</v>
+      </c>
+      <c r="R25">
+        <v>1.58371444271746</v>
+      </c>
+      <c r="S25">
+        <v>176.7101088664078</v>
+      </c>
+      <c r="T25">
+        <v>8.960670144513644</v>
+      </c>
+      <c r="U25">
+        <v>1001.161017035846</v>
+      </c>
+      <c r="V25">
+        <v>1.077759834778337</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
       <c r="A26" s="2">
         <v>43714.29166666666</v>
       </c>
@@ -1244,8 +2180,44 @@
       <c r="J26">
         <v>28.83110325532509</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26">
+        <v>1008.261572089</v>
+      </c>
+      <c r="L26">
+        <v>1.919750473619696</v>
+      </c>
+      <c r="M26">
+        <v>175.5372400857579</v>
+      </c>
+      <c r="N26">
+        <v>75.45373291509641</v>
+      </c>
+      <c r="O26">
+        <v>323.1962991141743</v>
+      </c>
+      <c r="P26">
+        <v>314.2747517334579</v>
+      </c>
+      <c r="Q26">
+        <v>61.68517600171822</v>
+      </c>
+      <c r="R26">
+        <v>0.6923288283588076</v>
+      </c>
+      <c r="S26">
+        <v>177.7125314999049</v>
+      </c>
+      <c r="T26">
+        <v>7.700657759043125</v>
+      </c>
+      <c r="U26">
+        <v>1000.578066472489</v>
+      </c>
+      <c r="V26">
+        <v>1.145211973929545</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22">
       <c r="A27" s="2">
         <v>43714.33333333334</v>
       </c>
@@ -1276,8 +2248,44 @@
       <c r="J27">
         <v>25.84390686380975</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27">
+        <v>1007.183727212009</v>
+      </c>
+      <c r="L27">
+        <v>32.25484295482447</v>
+      </c>
+      <c r="M27">
+        <v>147.645640148381</v>
+      </c>
+      <c r="N27">
+        <v>72.09227778903042</v>
+      </c>
+      <c r="O27">
+        <v>323.1845410495835</v>
+      </c>
+      <c r="P27">
+        <v>360.0782215661607</v>
+      </c>
+      <c r="Q27">
+        <v>59.20705745923406</v>
+      </c>
+      <c r="R27">
+        <v>1.441187213854897</v>
+      </c>
+      <c r="S27">
+        <v>166.7033615858207</v>
+      </c>
+      <c r="T27">
+        <v>6.439291098855355</v>
+      </c>
+      <c r="U27">
+        <v>1001.100340858082</v>
+      </c>
+      <c r="V27">
+        <v>0.6220323518893667</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22">
       <c r="A28" s="2">
         <v>43714.375</v>
       </c>
@@ -1308,8 +2316,44 @@
       <c r="J28">
         <v>29.38603616218032</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28">
+        <v>1006.254049328907</v>
+      </c>
+      <c r="L28">
+        <v>126.4488915049332</v>
+      </c>
+      <c r="M28">
+        <v>159.6584377846123</v>
+      </c>
+      <c r="N28">
+        <v>71.94988775999421</v>
+      </c>
+      <c r="O28">
+        <v>323.1336961224455</v>
+      </c>
+      <c r="P28">
+        <v>405.8712819007552</v>
+      </c>
+      <c r="Q28">
+        <v>55.77032484628444</v>
+      </c>
+      <c r="R28">
+        <v>1.049664599865789</v>
+      </c>
+      <c r="S28">
+        <v>151.3617210710607</v>
+      </c>
+      <c r="T28">
+        <v>5.54561507293142</v>
+      </c>
+      <c r="U28">
+        <v>1002.337000041115</v>
+      </c>
+      <c r="V28">
+        <v>0.8801297840984739</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29" s="2">
         <v>43714.41666666666</v>
       </c>
@@ -1340,8 +2384,44 @@
       <c r="J29">
         <v>24.96281367711322</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29">
+        <v>1005.79401863521</v>
+      </c>
+      <c r="L29">
+        <v>242.8912206997356</v>
+      </c>
+      <c r="M29">
+        <v>138.0430691727157</v>
+      </c>
+      <c r="N29">
+        <v>71.00669143507035</v>
+      </c>
+      <c r="O29">
+        <v>323.2135952936623</v>
+      </c>
+      <c r="P29">
+        <v>368.6629789492043</v>
+      </c>
+      <c r="Q29">
+        <v>56.34790900615972</v>
+      </c>
+      <c r="R29">
+        <v>1.777960435041436</v>
+      </c>
+      <c r="S29">
+        <v>137.8773121036588</v>
+      </c>
+      <c r="T29">
+        <v>5.064099461589899</v>
+      </c>
+      <c r="U29">
+        <v>1002.456336686175</v>
+      </c>
+      <c r="V29">
+        <v>1.207063005444907</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22">
       <c r="A30" s="2">
         <v>43714.45833333334</v>
       </c>
@@ -1372,8 +2452,44 @@
       <c r="J30">
         <v>27.4989716175034</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30">
+        <v>1008.156165188042</v>
+      </c>
+      <c r="L30">
+        <v>389.1071569150966</v>
+      </c>
+      <c r="M30">
+        <v>129.2915678737693</v>
+      </c>
+      <c r="N30">
+        <v>70.37114714843185</v>
+      </c>
+      <c r="O30">
+        <v>323.2014893586295</v>
+      </c>
+      <c r="P30">
+        <v>352.4476605964433</v>
+      </c>
+      <c r="Q30">
+        <v>60.26588607089089</v>
+      </c>
+      <c r="R30">
+        <v>1.527694017613744</v>
+      </c>
+      <c r="S30">
+        <v>162.890273231982</v>
+      </c>
+      <c r="T30">
+        <v>4.776425394002603</v>
+      </c>
+      <c r="U30">
+        <v>1002.548703015637</v>
+      </c>
+      <c r="V30">
+        <v>0.9241398203796768</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22">
       <c r="A31" s="2">
         <v>43714.5</v>
       </c>
@@ -1404,8 +2520,44 @@
       <c r="J31">
         <v>27.51875485451976</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31">
+        <v>1007.496690176181</v>
+      </c>
+      <c r="L31">
+        <v>580.8100463391306</v>
+      </c>
+      <c r="M31">
+        <v>154.4605221805357</v>
+      </c>
+      <c r="N31">
+        <v>70.27007910571396</v>
+      </c>
+      <c r="O31">
+        <v>322.8877063349447</v>
+      </c>
+      <c r="P31">
+        <v>364.8518570097695</v>
+      </c>
+      <c r="Q31">
+        <v>64.34483977079837</v>
+      </c>
+      <c r="R31">
+        <v>1.530189941516239</v>
+      </c>
+      <c r="S31">
+        <v>159.9162584291355</v>
+      </c>
+      <c r="T31">
+        <v>4.215198706395143</v>
+      </c>
+      <c r="U31">
+        <v>1001.48199832096</v>
+      </c>
+      <c r="V31">
+        <v>0.6513246303244489</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22">
       <c r="A32" s="2">
         <v>43714.54166666666</v>
       </c>
@@ -1436,8 +2588,44 @@
       <c r="J32">
         <v>26.54762139517486</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32">
+        <v>1007.555094299274</v>
+      </c>
+      <c r="L32">
+        <v>638.0579097553978</v>
+      </c>
+      <c r="M32">
+        <v>156.6027891425977</v>
+      </c>
+      <c r="N32">
+        <v>70.38498094131606</v>
+      </c>
+      <c r="O32">
+        <v>322.5618173762271</v>
+      </c>
+      <c r="P32">
+        <v>355.3083114412622</v>
+      </c>
+      <c r="Q32">
+        <v>67.04021315885953</v>
+      </c>
+      <c r="R32">
+        <v>1.309707390791903</v>
+      </c>
+      <c r="S32">
+        <v>144.5874140220467</v>
+      </c>
+      <c r="T32">
+        <v>3.705316332096783</v>
+      </c>
+      <c r="U32">
+        <v>1001.272021518524</v>
+      </c>
+      <c r="V32">
+        <v>0.6732634352331247</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22">
       <c r="A33" s="2">
         <v>43714.58333333334</v>
       </c>
@@ -1468,8 +2656,44 @@
       <c r="J33">
         <v>28.90111209618431</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33">
+        <v>1008.088625923241</v>
+      </c>
+      <c r="L33">
+        <v>630.834281339957</v>
+      </c>
+      <c r="M33">
+        <v>124.4691021341004</v>
+      </c>
+      <c r="N33">
+        <v>70.82309198115577</v>
+      </c>
+      <c r="O33">
+        <v>322.8877063349447</v>
+      </c>
+      <c r="P33">
+        <v>351.4952511066678</v>
+      </c>
+      <c r="Q33">
+        <v>67.96615290892359</v>
+      </c>
+      <c r="R33">
+        <v>1.853007649857711</v>
+      </c>
+      <c r="S33">
+        <v>173.7620855498768</v>
+      </c>
+      <c r="T33">
+        <v>3.270758093456856</v>
+      </c>
+      <c r="U33">
+        <v>1000.321541664701</v>
+      </c>
+      <c r="V33">
+        <v>0.5946032373439016</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22">
       <c r="A34" s="2">
         <v>43714.625</v>
       </c>
@@ -1500,8 +2724,44 @@
       <c r="J34">
         <v>29.27262137201028</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="K34">
+        <v>1006.99056725356</v>
+      </c>
+      <c r="L34">
+        <v>625.9587303055029</v>
+      </c>
+      <c r="M34">
+        <v>143.8754162236997</v>
+      </c>
+      <c r="N34">
+        <v>72.00563266938687</v>
+      </c>
+      <c r="O34">
+        <v>323.1724351145507</v>
+      </c>
+      <c r="P34">
+        <v>365.8064629212041</v>
+      </c>
+      <c r="Q34">
+        <v>68.56811357223199</v>
+      </c>
+      <c r="R34">
+        <v>0.931014525829666</v>
+      </c>
+      <c r="S34">
+        <v>198.9843349980915</v>
+      </c>
+      <c r="T34">
+        <v>2.639936109183028</v>
+      </c>
+      <c r="U34">
+        <v>1000.078388890324</v>
+      </c>
+      <c r="V34">
+        <v>0.3404181742696797</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22">
       <c r="A35" s="2">
         <v>43714.66666666666</v>
       </c>
@@ -1532,8 +2792,44 @@
       <c r="J35">
         <v>28.67430966266578</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="K35">
+        <v>1007.326991490984</v>
+      </c>
+      <c r="L35">
+        <v>570.9329314072083</v>
+      </c>
+      <c r="M35">
+        <v>97.17594476045386</v>
+      </c>
+      <c r="N35">
+        <v>73.31562192503455</v>
+      </c>
+      <c r="O35">
+        <v>322.7109596834653</v>
+      </c>
+      <c r="P35">
+        <v>363.9000084897114</v>
+      </c>
+      <c r="Q35">
+        <v>70.8748028882911</v>
+      </c>
+      <c r="R35">
+        <v>2.016444390888028</v>
+      </c>
+      <c r="S35">
+        <v>208.0388858193152</v>
+      </c>
+      <c r="T35">
+        <v>1.958157989218615</v>
+      </c>
+      <c r="U35">
+        <v>998.8871033738353</v>
+      </c>
+      <c r="V35">
+        <v>0.7201348294811798</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22">
       <c r="A36" s="2">
         <v>43714.70833333334</v>
       </c>
@@ -1564,8 +2860,44 @@
       <c r="J36">
         <v>26.92090658148536</v>
       </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="K36">
+        <v>1004.370185996583</v>
+      </c>
+      <c r="L36">
+        <v>430.5504520300469</v>
+      </c>
+      <c r="M36">
+        <v>147.6156361599494</v>
+      </c>
+      <c r="N36">
+        <v>73.25390298625058</v>
+      </c>
+      <c r="O36">
+        <v>322.6464325614259</v>
+      </c>
+      <c r="P36">
+        <v>358.1770238909215</v>
+      </c>
+      <c r="Q36">
+        <v>72.89571019694367</v>
+      </c>
+      <c r="R36">
+        <v>1.820273777729019</v>
+      </c>
+      <c r="S36">
+        <v>206.3715314225173</v>
+      </c>
+      <c r="T36">
+        <v>1.199482753631623</v>
+      </c>
+      <c r="U36">
+        <v>998.2985868328615</v>
+      </c>
+      <c r="V36">
+        <v>0.6967485059690944</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22">
       <c r="A37" s="2">
         <v>43714.75</v>
       </c>
@@ -1596,8 +2928,44 @@
       <c r="J37">
         <v>25.34049098893506</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="K37">
+        <v>1005.389589091516</v>
+      </c>
+      <c r="L37">
+        <v>222.7270605107492</v>
+      </c>
+      <c r="M37">
+        <v>164.3789549603515</v>
+      </c>
+      <c r="N37">
+        <v>72.32918552860049</v>
+      </c>
+      <c r="O37">
+        <v>322.6809596834653</v>
+      </c>
+      <c r="P37">
+        <v>393.4817812739651</v>
+      </c>
+      <c r="Q37">
+        <v>70.96113625354056</v>
+      </c>
+      <c r="R37">
+        <v>1.266417748861913</v>
+      </c>
+      <c r="S37">
+        <v>213.4059623504203</v>
+      </c>
+      <c r="T37">
+        <v>-0.1058334695137277</v>
+      </c>
+      <c r="U37">
+        <v>998.0530943336547</v>
+      </c>
+      <c r="V37">
+        <v>0.7668696356209963</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22">
       <c r="A38" s="2">
         <v>43714.79166666666</v>
       </c>
@@ -1628,8 +2996,44 @@
       <c r="J38">
         <v>27.0004013864165</v>
       </c>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="K38">
+        <v>1008.935759070606</v>
+      </c>
+      <c r="L38">
+        <v>79.95080207520977</v>
+      </c>
+      <c r="M38">
+        <v>168.160190042093</v>
+      </c>
+      <c r="N38">
+        <v>73.43410808771391</v>
+      </c>
+      <c r="O38">
+        <v>323.1458020574784</v>
+      </c>
+      <c r="P38">
+        <v>458.364129167233</v>
+      </c>
+      <c r="Q38">
+        <v>70.46234779871514</v>
+      </c>
+      <c r="R38">
+        <v>1.871450830697877</v>
+      </c>
+      <c r="S38">
+        <v>183.2236475656884</v>
+      </c>
+      <c r="T38">
+        <v>-1.658066411905037</v>
+      </c>
+      <c r="U38">
+        <v>999.3793540877236</v>
+      </c>
+      <c r="V38">
+        <v>0.7183847060003818</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22">
       <c r="A39" s="2">
         <v>43714.83333333334</v>
       </c>
@@ -1660,8 +3064,44 @@
       <c r="J39">
         <v>25.70312985118607</v>
       </c>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="K39">
+        <v>1010.410887858893</v>
+      </c>
+      <c r="L39">
+        <v>16.93166898367651</v>
+      </c>
+      <c r="M39">
+        <v>167.6071270548766</v>
+      </c>
+      <c r="N39">
+        <v>75.08134368208167</v>
+      </c>
+      <c r="O39">
+        <v>322.7935952936623</v>
+      </c>
+      <c r="P39">
+        <v>528.980993096834</v>
+      </c>
+      <c r="Q39">
+        <v>71.32218190549584</v>
+      </c>
+      <c r="R39">
+        <v>1.566977456979684</v>
+      </c>
+      <c r="S39">
+        <v>192.3392467884935</v>
+      </c>
+      <c r="T39">
+        <v>-3.24193509755062</v>
+      </c>
+      <c r="U39">
+        <v>998.4938837552571</v>
+      </c>
+      <c r="V39">
+        <v>0.6305055876406263</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
       <c r="A40" s="2">
         <v>43714.875</v>
       </c>
@@ -1692,8 +3132,44 @@
       <c r="J40">
         <v>27.06214150361209</v>
       </c>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="K40">
+        <v>1008.213486038652</v>
+      </c>
+      <c r="L40">
+        <v>-0.000589908447887403</v>
+      </c>
+      <c r="M40">
+        <v>118.0374296175598</v>
+      </c>
+      <c r="N40">
+        <v>76.12151825213409</v>
+      </c>
+      <c r="O40">
+        <v>322.7935952936623</v>
+      </c>
+      <c r="P40">
+        <v>406.8417055381606</v>
+      </c>
+      <c r="Q40">
+        <v>77.87136192718613</v>
+      </c>
+      <c r="R40">
+        <v>1.975278873498445</v>
+      </c>
+      <c r="S40">
+        <v>171.4122600936622</v>
+      </c>
+      <c r="T40">
+        <v>-4.235143031635299</v>
+      </c>
+      <c r="U40">
+        <v>998.0136041831182</v>
+      </c>
+      <c r="V40">
+        <v>0.9423495729295808</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22">
       <c r="A41" s="2">
         <v>43714.91666666666</v>
       </c>
@@ -1724,8 +3200,44 @@
       <c r="J41">
         <v>26.60078159105692</v>
       </c>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="K41">
+        <v>1008.195218973716</v>
+      </c>
+      <c r="L41">
+        <v>-0.0005284681001633718</v>
+      </c>
+      <c r="M41">
+        <v>114.9264301648923</v>
+      </c>
+      <c r="N41">
+        <v>76.92761012803983</v>
+      </c>
+      <c r="O41">
+        <v>323.1119054393864</v>
+      </c>
+      <c r="P41">
+        <v>336.2248416085596</v>
+      </c>
+      <c r="Q41">
+        <v>83.27535364124333</v>
+      </c>
+      <c r="R41">
+        <v>1.54607327420136</v>
+      </c>
+      <c r="S41">
+        <v>163.2895403928556</v>
+      </c>
+      <c r="T41">
+        <v>-5.047901302220977</v>
+      </c>
+      <c r="U41">
+        <v>998.2962482967141</v>
+      </c>
+      <c r="V41">
+        <v>1.351775554899279</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22">
       <c r="A42" s="2">
         <v>43714.95833333334</v>
       </c>
@@ -1756,8 +3268,44 @@
       <c r="J42">
         <v>27.74319065206485</v>
       </c>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="K42">
+        <v>1005.628852531491</v>
+      </c>
+      <c r="L42">
+        <v>-0.0005842184003800494</v>
+      </c>
+      <c r="M42">
+        <v>123.3775233040241</v>
+      </c>
+      <c r="N42">
+        <v>76.74811700925483</v>
+      </c>
+      <c r="O42">
+        <v>323.0997995043536</v>
+      </c>
+      <c r="P42">
+        <v>330.5018570097698</v>
+      </c>
+      <c r="Q42">
+        <v>83.50276004638647</v>
+      </c>
+      <c r="R42">
+        <v>1.251606418332973</v>
+      </c>
+      <c r="S42">
+        <v>154.0446832442908</v>
+      </c>
+      <c r="T42">
+        <v>-6.010429158915707</v>
+      </c>
+      <c r="U42">
+        <v>1000.272840368565</v>
+      </c>
+      <c r="V42">
+        <v>1.47817932606651</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22">
       <c r="A43" s="2">
         <v>43715</v>
       </c>
@@ -1788,8 +3336,44 @@
       <c r="J43">
         <v>26.67408377404088</v>
       </c>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="K43">
+        <v>1008.167932737392</v>
+      </c>
+      <c r="L43">
+        <v>-0.0005793120412909545</v>
+      </c>
+      <c r="M43">
+        <v>98.50882943552345</v>
+      </c>
+      <c r="N43">
+        <v>75.25254559914374</v>
+      </c>
+      <c r="O43">
+        <v>323.2135952936623</v>
+      </c>
+      <c r="P43">
+        <v>325.7305694594289</v>
+      </c>
+      <c r="Q43">
+        <v>82.20722685304253</v>
+      </c>
+      <c r="R43">
+        <v>1.892374306862286</v>
+      </c>
+      <c r="S43">
+        <v>144.5984164929869</v>
+      </c>
+      <c r="T43">
+        <v>-7.136059226298496</v>
+      </c>
+      <c r="U43">
+        <v>1000.815167559622</v>
+      </c>
+      <c r="V43">
+        <v>0.9814813585458035</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22">
       <c r="A44" s="2">
         <v>43715.04166666666</v>
       </c>
@@ -1820,8 +3404,44 @@
       <c r="J44">
         <v>28.26134985776875</v>
       </c>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="K44">
+        <v>1006.607094268481</v>
+      </c>
+      <c r="L44">
+        <v>-0.0004258422508686563</v>
+      </c>
+      <c r="M44">
+        <v>139.0121720878762</v>
+      </c>
+      <c r="N44">
+        <v>73.46776349679527</v>
+      </c>
+      <c r="O44">
+        <v>323.2135952936623</v>
+      </c>
+      <c r="P44">
+        <v>304.7435540582188</v>
+      </c>
+      <c r="Q44">
+        <v>79.24711270565865</v>
+      </c>
+      <c r="R44">
+        <v>1.140091173845528</v>
+      </c>
+      <c r="S44">
+        <v>176.793201053426</v>
+      </c>
+      <c r="T44">
+        <v>-8.223947805334742</v>
+      </c>
+      <c r="U44">
+        <v>999.9041936830785</v>
+      </c>
+      <c r="V44">
+        <v>0.7303627548549785</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
       <c r="A45" s="2">
         <v>43715.08333333334</v>
       </c>
@@ -1852,8 +3472,44 @@
       <c r="J45">
         <v>26.68500315585433</v>
       </c>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="K45">
+        <v>1005.74497777041</v>
+      </c>
+      <c r="L45">
+        <v>-0.0003191281233594927</v>
+      </c>
+      <c r="M45">
+        <v>143.9604019813453</v>
+      </c>
+      <c r="N45">
+        <v>72.27838827591538</v>
+      </c>
+      <c r="O45">
+        <v>323.2135952936623</v>
+      </c>
+      <c r="P45">
+        <v>301.8719327455743</v>
+      </c>
+      <c r="Q45">
+        <v>73.69269453883378</v>
+      </c>
+      <c r="R45">
+        <v>1.094961048318906</v>
+      </c>
+      <c r="S45">
+        <v>196.112980268578</v>
+      </c>
+      <c r="T45">
+        <v>-9.490466339924126</v>
+      </c>
+      <c r="U45">
+        <v>999.1510785753838</v>
+      </c>
+      <c r="V45">
+        <v>0.2004351920457358</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22">
       <c r="A46" s="2">
         <v>43715.125</v>
       </c>
@@ -1884,8 +3540,44 @@
       <c r="J46">
         <v>25.73956720602916</v>
       </c>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="K46">
+        <v>1005.659926885591</v>
+      </c>
+      <c r="L46">
+        <v>0.004065840432314495</v>
+      </c>
+      <c r="M46">
+        <v>156.0096718827544</v>
+      </c>
+      <c r="N46">
+        <v>73.49974130243046</v>
+      </c>
+      <c r="O46">
+        <v>323.2135952936623</v>
+      </c>
+      <c r="P46">
+        <v>292.3324179794871</v>
+      </c>
+      <c r="Q46">
+        <v>73.44492936063317</v>
+      </c>
+      <c r="R46">
+        <v>1.390638368845434</v>
+      </c>
+      <c r="S46">
+        <v>167.2511496095313</v>
+      </c>
+      <c r="T46">
+        <v>-10.3872231962619</v>
+      </c>
+      <c r="U46">
+        <v>999.554657427117</v>
+      </c>
+      <c r="V46">
+        <v>0.737187298184671</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22">
       <c r="A47" s="2">
         <v>43715.16666666666</v>
       </c>
@@ -1916,8 +3608,44 @@
       <c r="J47">
         <v>27.23222965834885</v>
       </c>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="K47">
+        <v>1005.626481585931</v>
+      </c>
+      <c r="L47">
+        <v>-0.0001634629977696238</v>
+      </c>
+      <c r="M47">
+        <v>145.3054270007486</v>
+      </c>
+      <c r="N47">
+        <v>74.98567696269116</v>
+      </c>
+      <c r="O47">
+        <v>323.2135952936623</v>
+      </c>
+      <c r="P47">
+        <v>282.7888724109798</v>
+      </c>
+      <c r="Q47">
+        <v>75.75059154375714</v>
+      </c>
+      <c r="R47">
+        <v>1.869401572496328</v>
+      </c>
+      <c r="S47">
+        <v>145.2283802816008</v>
+      </c>
+      <c r="T47">
+        <v>-11.21707301476294</v>
+      </c>
+      <c r="U47">
+        <v>999.8949713890293</v>
+      </c>
+      <c r="V47">
+        <v>1.096235034243356</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22">
       <c r="A48" s="2">
         <v>43715.20833333334</v>
       </c>
@@ -1948,8 +3676,44 @@
       <c r="J48">
         <v>29.66716199824666</v>
       </c>
-    </row>
-    <row r="49" spans="1:10">
+      <c r="K48">
+        <v>1007.291448307393</v>
+      </c>
+      <c r="L48">
+        <v>-8.897983290392669E-05</v>
+      </c>
+      <c r="M48">
+        <v>182.7396773866451</v>
+      </c>
+      <c r="N48">
+        <v>74.19382298105609</v>
+      </c>
+      <c r="O48">
+        <v>323.2135952936623</v>
+      </c>
+      <c r="P48">
+        <v>294.2388724109798</v>
+      </c>
+      <c r="Q48">
+        <v>75.54448944213446</v>
+      </c>
+      <c r="R48">
+        <v>1.069562510212124</v>
+      </c>
+      <c r="S48">
+        <v>135.9077979498386</v>
+      </c>
+      <c r="T48">
+        <v>-12.2954991640184</v>
+      </c>
+      <c r="U48">
+        <v>999.7523438432968</v>
+      </c>
+      <c r="V48">
+        <v>0.8433685901412387</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22">
       <c r="A49" s="2">
         <v>43715.25</v>
       </c>
@@ -1979,6 +3743,42 @@
       </c>
       <c r="J49">
         <v>26.96195097700461</v>
+      </c>
+      <c r="K49">
+        <v>1007.156846884228</v>
+      </c>
+      <c r="L49">
+        <v>-5.33117164079831E-05</v>
+      </c>
+      <c r="M49">
+        <v>131.4069426157315</v>
+      </c>
+      <c r="N49">
+        <v>77.53089863371768</v>
+      </c>
+      <c r="O49">
+        <v>323.2135952936623</v>
+      </c>
+      <c r="P49">
+        <v>374.4016298023561</v>
+      </c>
+      <c r="Q49">
+        <v>66.97718677560422</v>
+      </c>
+      <c r="R49">
+        <v>1.472862625779258</v>
+      </c>
+      <c r="S49">
+        <v>186.5841124561942</v>
+      </c>
+      <c r="T49">
+        <v>-14.02887809659089</v>
+      </c>
+      <c r="U49">
+        <v>999.7214474852655</v>
+      </c>
+      <c r="V49">
+        <v>0.8669820782245913</v>
       </c>
     </row>
   </sheetData>

</xml_diff>